<commit_message>
template audit simplifié accessible
</commit_message>
<xml_diff>
--- a/src/files/fr/general/template-grille-audit-simplifie.xlsx
+++ b/src/files/fr/general/template-grille-audit-simplifie.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IFI774\Projects\rgaa4lu\src\files\general\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sip\accessibilite.public.lu\src\files\fr\general\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F30AB2-7C59-4F7E-819A-F05D0D46959D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="10110" windowHeight="5340" tabRatio="861"/>
+    <workbookView xWindow="31500" yWindow="810" windowWidth="23040" windowHeight="14490" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Échantillon" sheetId="2" r:id="rId1"/>
@@ -25,8 +26,19 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Critères!$A$1:$C$54</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -550,7 +562,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
     <numFmt numFmtId="165" formatCode="0.000000%"/>
@@ -847,7 +859,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FF002060"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
@@ -1287,15 +1299,6 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1322,9 +1325,6 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1342,9 +1342,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1357,6 +1354,9 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1366,30 +1366,42 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="22">
-    <cellStyle name="cf1" xfId="15"/>
-    <cellStyle name="cf2" xfId="16"/>
-    <cellStyle name="cf3" xfId="17"/>
-    <cellStyle name="cf4" xfId="18"/>
-    <cellStyle name="cf5" xfId="19"/>
-    <cellStyle name="cf6" xfId="20"/>
-    <cellStyle name="Conforme" xfId="2"/>
-    <cellStyle name="Critère NA" xfId="3"/>
-    <cellStyle name="Dérogation" xfId="4"/>
-    <cellStyle name="Dérogation-N" xfId="5"/>
-    <cellStyle name="Entête tableau" xfId="6"/>
-    <cellStyle name="Heading1" xfId="7"/>
+    <cellStyle name="cf1" xfId="15" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="cf2" xfId="16" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="cf3" xfId="17" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="cf4" xfId="18" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="cf5" xfId="19" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="cf6" xfId="20" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Conforme" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Critère NA" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Dérogation" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Dérogation-N" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Entête tableau" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Heading1" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Non applicable" xfId="8"/>
-    <cellStyle name="Non conforme" xfId="9"/>
-    <cellStyle name="Non testé" xfId="10"/>
+    <cellStyle name="Non applicable" xfId="8" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Non conforme" xfId="9" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Non testé" xfId="10" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="21" builtinId="5"/>
-    <cellStyle name="Result" xfId="11"/>
-    <cellStyle name="Result2" xfId="12"/>
-    <cellStyle name="Titre tableau" xfId="13"/>
-    <cellStyle name="TitreViolet" xfId="14"/>
+    <cellStyle name="Result" xfId="11" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Result2" xfId="12" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Titre tableau" xfId="13" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="TitreViolet" xfId="14" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -1987,59 +1999,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.3046875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="39.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="68.88671875" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="7.33203125" style="15"/>
+    <col min="1" max="1" width="5.53515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="39.3046875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="68.84375" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="7.3046875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="85" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="85"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="83"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="79"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
@@ -2050,21 +2062,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="63"/>
       <c r="C8" s="64"/>
     </row>
-    <row r="9" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="63"/>
       <c r="C9" s="64"/>
     </row>
-    <row r="10" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>7</v>
       </c>
@@ -2088,67 +2100,67 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="18.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.23046875" customWidth="1"/>
+    <col min="3" max="3" width="17.765625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.765625" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="5.84375" customWidth="1"/>
+    <col min="9" max="9" width="7.23046875" customWidth="1"/>
+    <col min="10" max="10" width="8.765625" customWidth="1"/>
+    <col min="11" max="11" width="8.765625" style="3" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="6.69140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="D3" s="84" t="s">
+      <c r="B3" s="80"/>
+      <c r="D3" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="84"/>
+      <c r="E3" s="80"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="63" t="s">
         <v>113</v>
       </c>
@@ -2156,63 +2168,63 @@
         <f>Synthèse!B21</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="90" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="L4" s="78" t="s">
+      <c r="L4" s="93" t="s">
         <v>103</v>
       </c>
       <c r="M4" s="52" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="68">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D5" s="65">
         <f>Échantillon!B8</f>
         <v>0</v>
       </c>
-      <c r="E5" s="69" t="e">
+      <c r="E5" s="66" t="e">
         <f>BaseDeCalcul!E$74</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G5" s="70" t="s">
+      <c r="G5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="71">
+      <c r="H5" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G5, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G5, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5" s="68">
         <f t="shared" ref="J5:J17" si="0">H5+I5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="77">
+      <c r="K5" s="74">
         <f>IF(J5&gt;0, H5/J5, 0)*100</f>
         <v>0</v>
       </c>
-      <c r="L5" s="77" t="str">
+      <c r="L5" s="74" t="str">
         <f>IF(J5=0,"non applicable",IF(AND(K5&gt;=Échelle!$A$2, K5&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K5&gt;=Échelle!$A$3, K5&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K5&gt;=Échelle!$A$4, K5&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K5&gt;=Échelle!$A$5, K5&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K5&gt;=Échelle!$A$6, K5&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2221,35 +2233,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D6" s="68">
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="65">
         <f>Échantillon!B9</f>
         <v>0</v>
       </c>
-      <c r="E6" s="69" t="e">
+      <c r="E6" s="66" t="e">
         <f>BaseDeCalcul!F$74</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G6" s="70" t="s">
+      <c r="G6" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="71">
+      <c r="H6" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G6, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I6" s="71">
+      <c r="I6" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G6, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J6" s="71">
+      <c r="J6" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="77">
+      <c r="K6" s="74">
         <f t="shared" ref="K6:K17" si="1">IF(J6&gt;0, H6/J6, 0)*100</f>
         <v>0</v>
       </c>
-      <c r="L6" s="77" t="str">
+      <c r="L6" s="74" t="str">
         <f>IF(J6=0,"non applicable",IF(AND(K6&gt;=Échelle!$A$2, K6&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K6&gt;=Échelle!$A$3, K6&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K6&gt;=Échelle!$A$4, K6&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K6&gt;=Échelle!$A$5, K6&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K6&gt;=Échelle!$A$6, K6&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2258,37 +2270,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
-      <c r="D7" s="73">
+      <c r="D7" s="70">
         <f>Échantillon!B10</f>
         <v>0</v>
       </c>
-      <c r="E7" s="74" t="e">
+      <c r="E7" s="71" t="e">
         <f>BaseDeCalcul!G$74</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G7" s="70" t="s">
+      <c r="G7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="71">
+      <c r="H7" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G7, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G7, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J7" s="71">
+      <c r="J7" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="77">
+      <c r="K7" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="77" t="str">
+      <c r="L7" s="74" t="str">
         <f>IF(J7=0,"non applicable",IF(AND(K7&gt;=Échelle!$A$2, K7&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K7&gt;=Échelle!$A$3, K7&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K7&gt;=Échelle!$A$4, K7&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K7&gt;=Échelle!$A$5, K7&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K7&gt;=Échelle!$A$6, K7&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2297,57 +2309,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G8" s="72" t="s">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G8, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I8" s="71">
+      <c r="I8" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G8, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J8" s="71">
+      <c r="J8" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K8" s="77">
+      <c r="K8" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="77" t="str">
+      <c r="L8" s="74" t="str">
         <f>IF(J8=0,"non applicable",IF(AND(K8&gt;=Échelle!$A$2, K8&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K8&gt;=Échelle!$A$3, K8&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K8&gt;=Échelle!$A$4, K8&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K8&gt;=Échelle!$A$5, K8&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K8&gt;=Échelle!$A$6, K8&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
       <c r="M8" s="55"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="58"/>
       <c r="C9" s="59"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="G9" s="72" t="s">
+      <c r="G9" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="71">
+      <c r="H9" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G9, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I9" s="71">
+      <c r="I9" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G9, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J9" s="71">
+      <c r="J9" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="77">
+      <c r="K9" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="77" t="str">
+      <c r="L9" s="74" t="str">
         <f>IF(J9=0,"non applicable",IF(AND(K9&gt;=Échelle!$A$2, K9&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K9&gt;=Échelle!$A$3, K9&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K9&gt;=Échelle!$A$4, K9&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K9&gt;=Échelle!$A$5, K9&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K9&gt;=Échelle!$A$6, K9&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2356,32 +2368,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="58"/>
       <c r="B10" s="3"/>
       <c r="C10" s="59"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="G10" s="72" t="s">
+      <c r="G10" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="71">
+      <c r="H10" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G10, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I10" s="71">
+      <c r="I10" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G10, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J10" s="71">
+      <c r="J10" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K10" s="77">
+      <c r="K10" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L10" s="77" t="str">
+      <c r="L10" s="74" t="str">
         <f>IF(J10=0,"non applicable",IF(AND(K10&gt;=Échelle!$A$2, K10&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K10&gt;=Échelle!$A$3, K10&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K10&gt;=Échelle!$A$4, K10&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K10&gt;=Échelle!$A$5, K10&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K10&gt;=Échelle!$A$6, K10&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2390,29 +2402,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="G11" s="72" t="s">
+      <c r="G11" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="71">
+      <c r="H11" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G11, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I11" s="71">
+      <c r="I11" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G11, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J11" s="71">
+      <c r="J11" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K11" s="77">
+      <c r="K11" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L11" s="77" t="str">
+      <c r="L11" s="74" t="str">
         <f>IF(J11=0,"non applicable",IF(AND(K11&gt;=Échelle!$A$2, K11&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K11&gt;=Échelle!$A$3, K11&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K11&gt;=Échelle!$A$4, K11&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K11&gt;=Échelle!$A$5, K11&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K11&gt;=Échelle!$A$6, K11&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2421,27 +2433,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G12" s="72" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G12" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="71">
+      <c r="H12" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G12, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I12" s="71">
+      <c r="I12" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G12, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J12" s="71">
+      <c r="J12" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K12" s="77">
+      <c r="K12" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L12" s="77" t="str">
+      <c r="L12" s="74" t="str">
         <f>IF(J12=0,"non applicable",IF(AND(K12&gt;=Échelle!$A$2, K12&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K12&gt;=Échelle!$A$3, K12&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K12&gt;=Échelle!$A$4, K12&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K12&gt;=Échelle!$A$5, K12&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K12&gt;=Échelle!$A$6, K12&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2450,27 +2462,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G13" s="72" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G13" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="71">
+      <c r="H13" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G13, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I13" s="71">
+      <c r="I13" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G13, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J13" s="71">
+      <c r="J13" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K13" s="77">
+      <c r="K13" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L13" s="77" t="str">
+      <c r="L13" s="74" t="str">
         <f>IF(J13=0,"non applicable",IF(AND(K13&gt;=Échelle!$A$2, K13&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K13&gt;=Échelle!$A$3, K13&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K13&gt;=Échelle!$A$4, K13&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K13&gt;=Échelle!$A$5, K13&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K13&gt;=Échelle!$A$6, K13&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2479,27 +2491,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G14" s="72" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G14" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="71">
+      <c r="H14" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G14, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I14" s="71">
+      <c r="I14" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G14, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J14" s="71">
+      <c r="J14" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K14" s="77">
+      <c r="K14" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14" s="77" t="str">
+      <c r="L14" s="74" t="str">
         <f>IF(J14=0,"non applicable",IF(AND(K14&gt;=Échelle!$A$2, K14&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K14&gt;=Échelle!$A$3, K14&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K14&gt;=Échelle!$A$4, K14&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K14&gt;=Échelle!$A$5, K14&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K14&gt;=Échelle!$A$6, K14&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2508,27 +2520,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G15" s="72" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G15" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="71">
+      <c r="H15" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G15, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I15" s="71">
+      <c r="I15" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G15, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J15" s="71">
+      <c r="J15" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K15" s="77">
+      <c r="K15" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15" s="77" t="str">
+      <c r="L15" s="74" t="str">
         <f>IF(J15=0,"non applicable",IF(AND(K15&gt;=Échelle!$A$2, K15&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K15&gt;=Échelle!$A$3, K15&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K15&gt;=Échelle!$A$4, K15&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K15&gt;=Échelle!$A$5, K15&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K15&gt;=Échelle!$A$6, K15&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2537,27 +2549,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G16" s="72" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G16" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="71">
+      <c r="H16" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G16, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I16" s="71">
+      <c r="I16" s="68">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G16, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J16" s="71">
+      <c r="J16" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K16" s="77">
+      <c r="K16" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L16" s="77" t="str">
+      <c r="L16" s="74" t="str">
         <f>IF(J16=0,"non applicable",IF(AND(K16&gt;=Échelle!$A$2, K16&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K16&gt;=Échelle!$A$3, K16&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K16&gt;=Échelle!$A$4, K16&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K16&gt;=Échelle!$A$5, K16&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K16&gt;=Échelle!$A$6, K16&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2566,27 +2578,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G17" s="75" t="s">
+    <row r="17" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G17" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="76">
+      <c r="H17" s="73">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G17, BaseDeCalcul!L$3:L$66, "C")</f>
         <v>0</v>
       </c>
-      <c r="I17" s="76">
+      <c r="I17" s="73">
         <f>COUNTIFS(BaseDeCalcul!C$3:C$66, G17, BaseDeCalcul!L$3:L$66, "NC")</f>
         <v>0</v>
       </c>
-      <c r="J17" s="76">
+      <c r="J17" s="73">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K17" s="77">
+      <c r="K17" s="74">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L17" s="77" t="str">
+      <c r="L17" s="74" t="str">
         <f>IF(J17=0,"non applicable",IF(AND(K17&gt;=Échelle!$A$2, K17&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(K17&gt;=Échelle!$A$3, K17&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(K17&gt;=Échelle!$A$4, K17&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(K17&gt;=Échelle!$A$5, K17&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(K17&gt;=Échelle!$A$6, K17&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) ))</f>
         <v>non applicable</v>
       </c>
@@ -2595,16 +2607,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M18" s="55">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
     </row>
   </sheetData>
@@ -2620,25 +2632,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BL54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="76.77734375" style="5" customWidth="1"/>
-    <col min="4" max="5" width="9.5546875" style="5"/>
-    <col min="6" max="6" width="9.5546875" style="1"/>
-    <col min="7" max="64" width="9.5546875" style="5"/>
-    <col min="1024" max="1024" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.3046875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="76.765625" style="5" customWidth="1"/>
+    <col min="4" max="5" width="9.53515625" style="5"/>
+    <col min="6" max="6" width="9.53515625" style="1"/>
+    <col min="7" max="64" width="9.53515625" style="5"/>
+    <col min="1024" max="1024" width="7.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="86" t="str">
         <f>Échantillon!A1</f>
         <v>AUDIT SIMPLIFIÉ – GRILLE D'ÉVALUATION</v>
@@ -2646,7 +2658,7 @@
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
     </row>
-    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>8</v>
       </c>
@@ -2657,8 +2669,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="87" t="s">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="82" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="62" t="s">
@@ -2669,8 +2681,8 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="87"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="82"/>
       <c r="B4" s="62" t="s">
         <v>13</v>
       </c>
@@ -2679,8 +2691,8 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="82"/>
       <c r="B5" s="62" t="s">
         <v>14</v>
       </c>
@@ -2689,8 +2701,8 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="82"/>
       <c r="B6" s="62" t="s">
         <v>16</v>
       </c>
@@ -2699,8 +2711,8 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="82"/>
       <c r="B7" s="62" t="s">
         <v>17</v>
       </c>
@@ -2709,8 +2721,8 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="87"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="82"/>
       <c r="B8" s="62" t="s">
         <v>18</v>
       </c>
@@ -2719,8 +2731,8 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="87"/>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="82"/>
       <c r="B9" s="62" t="s">
         <v>19</v>
       </c>
@@ -2729,7 +2741,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" ht="41.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="41" x14ac:dyDescent="0.35">
       <c r="A10" s="60" t="s">
         <v>20</v>
       </c>
@@ -2741,8 +2753,8 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="87" t="s">
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="82" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="62" t="s">
@@ -2753,8 +2765,8 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="87"/>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="82"/>
       <c r="B12" s="62" t="s">
         <v>23</v>
       </c>
@@ -2763,8 +2775,8 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="87" t="s">
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="82" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="62" t="s">
@@ -2775,8 +2787,8 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="87"/>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="82"/>
       <c r="B14" s="62" t="s">
         <v>26</v>
       </c>
@@ -2785,8 +2797,8 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="87"/>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="82"/>
       <c r="B15" s="62" t="s">
         <v>27</v>
       </c>
@@ -2795,8 +2807,8 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="87"/>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="82"/>
       <c r="B16" s="62" t="s">
         <v>28</v>
       </c>
@@ -2805,8 +2817,8 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="87"/>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A17" s="82"/>
       <c r="B17" s="62" t="s">
         <v>29</v>
       </c>
@@ -2815,8 +2827,8 @@
       </c>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="87"/>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A18" s="82"/>
       <c r="B18" s="62" t="s">
         <v>30</v>
       </c>
@@ -2825,8 +2837,8 @@
       </c>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="87"/>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A19" s="82"/>
       <c r="B19" s="62" t="s">
         <v>31</v>
       </c>
@@ -2835,8 +2847,8 @@
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="87"/>
+    <row r="20" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="82"/>
       <c r="B20" s="62" t="s">
         <v>32</v>
       </c>
@@ -2845,8 +2857,8 @@
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="87" t="s">
+    <row r="21" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="82" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="62" t="s">
@@ -2857,8 +2869,8 @@
       </c>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="87"/>
+    <row r="22" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="82"/>
       <c r="B22" s="62" t="s">
         <v>35</v>
       </c>
@@ -2867,8 +2879,8 @@
       </c>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:64" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="87" t="s">
+    <row r="23" spans="1:64" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="82" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="62" t="s">
@@ -2879,8 +2891,8 @@
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:64" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="87"/>
+    <row r="24" spans="1:64" ht="22.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="82"/>
       <c r="B24" s="62" t="s">
         <v>38</v>
       </c>
@@ -2889,7 +2901,7 @@
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:64" ht="42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" ht="41.5" x14ac:dyDescent="0.35">
       <c r="A25" s="60" t="s">
         <v>39</v>
       </c>
@@ -2901,8 +2913,8 @@
       </c>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="88" t="s">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="83" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="32" t="s">
@@ -2972,8 +2984,8 @@
       <c r="BK26" s="5"/>
       <c r="BL26" s="5"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="89"/>
+    <row r="27" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="84"/>
       <c r="B27" s="32" t="s">
         <v>100</v>
       </c>
@@ -3041,8 +3053,8 @@
       <c r="BK27" s="5"/>
       <c r="BL27" s="5"/>
     </row>
-    <row r="28" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="89"/>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A28" s="84"/>
       <c r="B28" s="62" t="s">
         <v>42</v>
       </c>
@@ -3051,8 +3063,8 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="89"/>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A29" s="84"/>
       <c r="B29" s="62" t="s">
         <v>43</v>
       </c>
@@ -3061,8 +3073,8 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="89"/>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A30" s="84"/>
       <c r="B30" s="62" t="s">
         <v>44</v>
       </c>
@@ -3071,8 +3083,8 @@
       </c>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="89"/>
+    <row r="31" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="84"/>
       <c r="B31" s="62" t="s">
         <v>45</v>
       </c>
@@ -3081,8 +3093,8 @@
       </c>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:64" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="90"/>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A32" s="85"/>
       <c r="B32" s="62" t="s">
         <v>46</v>
       </c>
@@ -3091,8 +3103,8 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="87" t="s">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="82" t="s">
         <v>47</v>
       </c>
       <c r="B33" s="62" t="s">
@@ -3103,8 +3115,8 @@
       </c>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="87"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="82"/>
       <c r="B34" s="62" t="s">
         <v>49</v>
       </c>
@@ -3113,8 +3125,8 @@
       </c>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="87" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="82" t="s">
         <v>50</v>
       </c>
       <c r="B35" s="62" t="s">
@@ -3125,8 +3137,8 @@
       </c>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="87"/>
+    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="82"/>
       <c r="B36" s="62" t="s">
         <v>52</v>
       </c>
@@ -3135,8 +3147,8 @@
       </c>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="87"/>
+    <row r="37" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="82"/>
       <c r="B37" s="62" t="s">
         <v>53</v>
       </c>
@@ -3145,8 +3157,8 @@
       </c>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" s="87"/>
+    <row r="38" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="82"/>
       <c r="B38" s="62" t="s">
         <v>54</v>
       </c>
@@ -3155,8 +3167,8 @@
       </c>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="87"/>
+    <row r="39" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="82"/>
       <c r="B39" s="62" t="s">
         <v>55</v>
       </c>
@@ -3165,8 +3177,8 @@
       </c>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="87" t="s">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="82" t="s">
         <v>56</v>
       </c>
       <c r="B40" s="62" t="s">
@@ -3177,8 +3189,8 @@
       </c>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="87"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="82"/>
       <c r="B41" s="62" t="s">
         <v>58</v>
       </c>
@@ -3187,8 +3199,8 @@
       </c>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="87"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="82"/>
       <c r="B42" s="62" t="s">
         <v>59</v>
       </c>
@@ -3197,8 +3209,8 @@
       </c>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="87"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="82"/>
       <c r="B43" s="62" t="s">
         <v>60</v>
       </c>
@@ -3207,8 +3219,8 @@
       </c>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="87"/>
+    <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="82"/>
       <c r="B44" s="62" t="s">
         <v>61</v>
       </c>
@@ -3217,8 +3229,8 @@
       </c>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="87"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="82"/>
       <c r="B45" s="62" t="s">
         <v>62</v>
       </c>
@@ -3227,8 +3239,8 @@
       </c>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="87"/>
+    <row r="46" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="82"/>
       <c r="B46" s="62" t="s">
         <v>63</v>
       </c>
@@ -3237,8 +3249,8 @@
       </c>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.2">
-      <c r="A47" s="87" t="s">
+    <row r="47" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="82" t="s">
         <v>64</v>
       </c>
       <c r="B47" s="62" t="s">
@@ -3249,8 +3261,8 @@
       </c>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" s="87"/>
+    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A48" s="82"/>
       <c r="B48" s="62" t="s">
         <v>66</v>
       </c>
@@ -3259,8 +3271,8 @@
       </c>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="87"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="82"/>
       <c r="B49" s="62" t="s">
         <v>67</v>
       </c>
@@ -3269,8 +3281,8 @@
       </c>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="87"/>
+    <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A50" s="82"/>
       <c r="B50" s="62" t="s">
         <v>68</v>
       </c>
@@ -3279,8 +3291,8 @@
       </c>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A51" s="87"/>
+    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="82"/>
       <c r="B51" s="62" t="s">
         <v>69</v>
       </c>
@@ -3289,8 +3301,8 @@
       </c>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A52" s="87" t="s">
+    <row r="52" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="82" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="62" t="s">
@@ -3301,8 +3313,8 @@
       </c>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A53" s="87"/>
+    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="82"/>
       <c r="B53" s="62" t="s">
         <v>72</v>
       </c>
@@ -3311,8 +3323,8 @@
       </c>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="87"/>
+    <row r="54" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="82"/>
       <c r="B54" s="62" t="s">
         <v>73</v>
       </c>
@@ -3323,6 +3335,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A35:A39"/>
     <mergeCell ref="A40:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A54"/>
@@ -3330,11 +3347,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.53263888888888899" bottom="0.39374999999999999" header="0.39374999999999999" footer="0.39374999999999999"/>
   <pageSetup scale="74" pageOrder="overThenDown" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3345,154 +3357,154 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R119"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.3046875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="10.53515625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="5.69140625" style="15" customWidth="1"/>
     <col min="3" max="12" width="5" style="22" customWidth="1"/>
     <col min="13" max="13" width="5" style="15" customWidth="1"/>
-    <col min="14" max="14" width="4.21875" style="15" customWidth="1"/>
-    <col min="15" max="15" width="4.77734375" style="15" customWidth="1"/>
-    <col min="16" max="16" width="1.77734375" style="15" customWidth="1"/>
-    <col min="17" max="17" width="4.88671875" style="15" customWidth="1"/>
-    <col min="18" max="18" width="5.77734375" style="15" customWidth="1"/>
-    <col min="19" max="16384" width="7.33203125" style="15"/>
+    <col min="14" max="14" width="4.23046875" style="15" customWidth="1"/>
+    <col min="15" max="15" width="4.765625" style="15" customWidth="1"/>
+    <col min="16" max="16" width="1.765625" style="15" customWidth="1"/>
+    <col min="17" max="17" width="4.84375" style="15" customWidth="1"/>
+    <col min="18" max="18" width="5.765625" style="15" customWidth="1"/>
+    <col min="19" max="16384" width="7.3046875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="84" t="str">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="80" t="str">
         <f>Échantillon!A1</f>
         <v>AUDIT SIMPLIFIÉ – GRILLE D'ÉVALUATION</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="92" t="s">
+      <c r="D3" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="92" t="s">
+      <c r="E3" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="88" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="92" t="s">
+      <c r="I3" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="92" t="s">
+      <c r="K3" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="92" t="s">
+      <c r="L3" s="88" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="92" t="s">
+      <c r="M3" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="92" t="s">
+      <c r="N3" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="92" t="s">
+      <c r="O3" s="88" t="s">
         <v>70</v>
       </c>
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="34"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="19"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="92"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="34"/>
       <c r="R4" s="34"/>
     </row>
-    <row r="5" spans="1:18" ht="59.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="59.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
       <c r="P5" s="34"/>
       <c r="Q5" s="34"/>
       <c r="R5" s="34"/>
     </row>
-    <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="35" t="s">
         <v>76</v>
       </c>
@@ -3557,7 +3569,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
       <c r="B7" s="38" t="s">
         <v>77</v>
@@ -3623,7 +3635,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="20"/>
       <c r="B8" s="41" t="s">
         <v>78</v>
@@ -3689,7 +3701,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="20"/>
       <c r="B9" s="44" t="s">
         <v>79</v>
@@ -3755,7 +3767,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20"/>
       <c r="B10" s="44" t="s">
         <v>80</v>
@@ -3821,7 +3833,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -3837,162 +3849,162 @@
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B14" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B15" s="57" t="str">
         <f>IF(Q10=0,ROUND(COUNTIF(BaseDeCalcul!L3:L66,"C")/(COUNTIF(BaseDeCalcul!L3:L66,"C")+COUNTIF(BaseDeCalcul!L3:L66,"NC"))*100, 2)&amp;"%","Pourcentage indisponible : il reste "&amp;Q10&amp;" critère(s) NT.")</f>
         <v>Pourcentage indisponible : il reste 156 critère(s) NT.</v>
       </c>
       <c r="C15" s="23"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C16" s="23"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="str">
         <f>IF(Q10=0,ROUND(AVERAGEIF(BaseDeCalcul!E71:G71,"&lt;&gt;NA")*100,1)&amp;"%","Pourcentage indisponible : il reste "&amp;Q10&amp;" critère(s) NT.")</f>
         <v>Pourcentage indisponible : il reste 156 critère(s) NT.</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="e">
         <f>B15*100</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="15" t="e">
         <f>IF(AND(Synthèse!B20&gt;=Échelle!A2, Synthèse!B20&lt;Échelle!B2), Échelle!C2, IF(AND(Synthèse!B20&gt;=Échelle!A3, Synthèse!B20&lt;Échelle!B3), Échelle!C3, IF(AND(Synthèse!B20&gt;=Échelle!A4, Synthèse!B20&lt;Échelle!B4), Échelle!C4, IF(AND(Synthèse!B20&gt;=Échelle!A5, Synthèse!B20&lt;Échelle!B5), Échelle!C5, IF(AND(Synthèse!B20&gt;=Échelle!A6, Synthèse!B20&lt;=Échelle!B6), Échelle!C6, "" ) ) ) ) )</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119" s="22">
         <v>1</v>
       </c>
@@ -4025,31 +4037,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE74"/>
   <sheetViews>
     <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="5.5546875" style="7" customWidth="1"/>
-    <col min="8" max="11" width="5.109375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" style="1"/>
-    <col min="13" max="14" width="5.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="22.77734375" style="1" customWidth="1"/>
-    <col min="16" max="18" width="5.5546875" style="7" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" style="8" customWidth="1"/>
-    <col min="20" max="31" width="9.5546875" style="1"/>
-    <col min="991" max="991" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.3046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.3046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="5.53515625" style="7" customWidth="1"/>
+    <col min="8" max="11" width="5.07421875" style="8" customWidth="1"/>
+    <col min="12" max="12" width="9.53515625" style="1"/>
+    <col min="13" max="14" width="5.3046875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="22.765625" style="1" customWidth="1"/>
+    <col min="16" max="18" width="5.53515625" style="7" customWidth="1"/>
+    <col min="19" max="19" width="7.3046875" style="8" customWidth="1"/>
+    <col min="20" max="31" width="9.53515625" style="1"/>
+    <col min="991" max="991" width="7.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="D1" s="3" t="s">
         <v>95</v>
       </c>
@@ -4087,7 +4099,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -4118,7 +4130,7 @@
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -4193,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="15">
         <v>1</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="15">
         <v>1</v>
       </c>
@@ -4343,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="15">
         <v>1</v>
       </c>
@@ -4418,7 +4430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="15">
         <v>1</v>
       </c>
@@ -4493,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>1</v>
       </c>
@@ -4568,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="15">
         <v>1</v>
       </c>
@@ -4643,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="25"/>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -4679,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -4754,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="25"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -4790,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="15">
         <v>3</v>
       </c>
@@ -4865,7 +4877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="15">
         <v>3</v>
       </c>
@@ -4940,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="25"/>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
@@ -4976,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="15">
         <v>4</v>
       </c>
@@ -5051,7 +5063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="15">
         <v>4</v>
       </c>
@@ -5126,7 +5138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="15">
         <v>4</v>
       </c>
@@ -5201,7 +5213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="15">
         <v>4</v>
       </c>
@@ -5276,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="15">
         <v>4</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="15">
         <v>4</v>
       </c>
@@ -5426,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="15">
         <v>4</v>
       </c>
@@ -5501,7 +5513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="15">
         <v>4</v>
       </c>
@@ -5576,7 +5588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="25"/>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -5612,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="15">
         <v>5</v>
       </c>
@@ -5687,7 +5699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="15">
         <v>5</v>
       </c>
@@ -5762,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="25"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -5798,7 +5810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="15">
         <v>6</v>
       </c>
@@ -5873,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="15">
         <v>6</v>
       </c>
@@ -5948,7 +5960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="25"/>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -5984,7 +5996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="15">
         <v>7</v>
       </c>
@@ -6059,7 +6071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="25"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -6095,7 +6107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="15">
         <v>8</v>
       </c>
@@ -6168,7 +6180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="15">
         <v>8</v>
       </c>
@@ -6241,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="15">
         <v>8</v>
       </c>
@@ -6316,7 +6328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="15">
         <v>8</v>
       </c>
@@ -6391,7 +6403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="15">
         <v>8</v>
       </c>
@@ -6466,7 +6478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="15">
         <v>8</v>
       </c>
@@ -6541,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="15">
         <v>8</v>
       </c>
@@ -6616,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="25"/>
       <c r="B40" s="26"/>
       <c r="C40" s="26"/>
@@ -6652,7 +6664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="15">
         <v>9</v>
       </c>
@@ -6727,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="15">
         <v>9</v>
       </c>
@@ -6802,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="25"/>
       <c r="B43" s="26"/>
       <c r="C43" s="26"/>
@@ -6838,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="15">
         <v>10</v>
       </c>
@@ -6913,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="15">
         <v>10</v>
       </c>
@@ -6988,7 +7000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="15">
         <v>10</v>
       </c>
@@ -7063,7 +7075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="15">
         <v>10</v>
       </c>
@@ -7138,7 +7150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="15">
         <v>10</v>
       </c>
@@ -7213,7 +7225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="25"/>
       <c r="B49" s="26"/>
       <c r="C49" s="26"/>
@@ -7249,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="15">
         <v>11</v>
       </c>
@@ -7324,7 +7336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="15">
         <v>11</v>
       </c>
@@ -7399,7 +7411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="15">
         <v>11</v>
       </c>
@@ -7474,7 +7486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="15">
         <v>11</v>
       </c>
@@ -7549,7 +7561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <v>11</v>
       </c>
@@ -7624,7 +7636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="15">
         <v>11</v>
       </c>
@@ -7699,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="15">
         <v>11</v>
       </c>
@@ -7774,7 +7786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="25"/>
       <c r="B57" s="26"/>
       <c r="C57" s="26"/>
@@ -7810,7 +7822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="15">
         <v>12</v>
       </c>
@@ -7885,7 +7897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="15">
         <v>12</v>
       </c>
@@ -7960,7 +7972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="15">
         <v>12</v>
       </c>
@@ -8035,7 +8047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <v>12</v>
       </c>
@@ -8110,7 +8122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="15">
         <v>12</v>
       </c>
@@ -8185,7 +8197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="25"/>
       <c r="B63" s="26"/>
       <c r="C63" s="26"/>
@@ -8221,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="15">
         <v>13</v>
       </c>
@@ -8296,7 +8308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A65" s="15">
         <v>13</v>
       </c>
@@ -8371,7 +8383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A66" s="15">
         <v>13</v>
       </c>
@@ -8446,7 +8458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A67" s="25"/>
       <c r="B67" s="26"/>
       <c r="C67" s="26"/>
@@ -8482,7 +8494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A68" s="15"/>
       <c r="B68" s="22"/>
       <c r="C68" s="22" t="s">
@@ -8526,7 +8538,7 @@
       <c r="AD68" s="3"/>
       <c r="AE68" s="3"/>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A69" s="15"/>
       <c r="B69" s="22"/>
       <c r="C69" s="22" t="s">
@@ -8570,7 +8582,7 @@
       <c r="AD69" s="3"/>
       <c r="AE69" s="3"/>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A70" s="15"/>
       <c r="B70" s="22"/>
       <c r="C70" s="22" t="s">
@@ -8614,7 +8626,7 @@
       <c r="AD70" s="3"/>
       <c r="AE70" s="3"/>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" s="15"/>
       <c r="B71" s="22"/>
       <c r="C71" s="22" t="s">
@@ -8661,7 +8673,7 @@
       <c r="AD71" s="3"/>
       <c r="AE71" s="3"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
       <c r="E73" s="7" t="e">
         <f>E71*100</f>
         <v>#VALUE!</v>
@@ -8675,7 +8687,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.35">
       <c r="E74" s="7" t="e">
         <f>IF(AND(E73&gt;=Échelle!$A$2, E73&lt;Échelle!$B$2), Échelle!$C$2, IF(AND(E73&gt;=Échelle!$A$3, E73&lt;Échelle!$B$3), Échelle!$C$3, IF(AND(E73&gt;=Échelle!$A$4, E73&lt;Échelle!$B$4), Échelle!$C$4, IF(AND(E73&gt;=Échelle!$A$5, E73&lt;Échelle!$B$5), Échelle!$C$5, IF(AND(E73&gt;=Échelle!$A$6, E73&lt;=Échelle!$B$6), Échelle!$C$6, "" ) ) ) ) )</f>
         <v>#VALUE!</v>
@@ -8699,19 +8711,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.77734375" style="3"/>
+    <col min="1" max="2" width="8.765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>106</v>
       </c>
@@ -8722,7 +8734,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -8733,7 +8745,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -8744,7 +8756,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>40</v>
       </c>
@@ -8755,7 +8767,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>60</v>
       </c>
@@ -8766,7 +8778,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>80</v>
       </c>
@@ -8784,51 +8796,51 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMI55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="39.88671875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="79.77734375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="5" customWidth="1"/>
-    <col min="8" max="64" width="9.5546875" style="5"/>
-    <col min="1024" max="1024" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.69140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="39.84375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="3.765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3.23046875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="79.765625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.84375" style="5" customWidth="1"/>
+    <col min="8" max="64" width="9.53515625" style="5"/>
+    <col min="1024" max="1024" width="7.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1023" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="str">
+    <row r="1" spans="1:1023" x14ac:dyDescent="0.35">
+      <c r="A1" s="80" t="str">
         <f>Échantillon!A1</f>
         <v>AUDIT SIMPLIFIÉ – GRILLE D'ÉVALUATION</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-    </row>
-    <row r="2" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="str">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+    </row>
+    <row r="2" spans="1:1023" x14ac:dyDescent="0.35">
+      <c r="A2" s="89" t="str">
         <f>CONCATENATE(Échantillon!B8," : ",Échantillon!C8)</f>
         <v xml:space="preserve"> : </v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-    </row>
-    <row r="3" spans="1:1023" ht="61.5" x14ac:dyDescent="0.2">
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+    </row>
+    <row r="3" spans="1:1023" ht="61.5" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
@@ -8908,8 +8920,8 @@
       <c r="BK3" s="2"/>
       <c r="BL3" s="2"/>
     </row>
-    <row r="4" spans="1:1023" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="str">
+    <row r="4" spans="1:1023" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="82" t="str">
         <f>Critères!$A$3</f>
         <v>IMAGES</v>
       </c>
@@ -8987,8 +8999,8 @@
       <c r="BK4" s="2"/>
       <c r="BL4" s="2"/>
     </row>
-    <row r="5" spans="1:1023" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
+    <row r="5" spans="1:1023" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="82"/>
       <c r="B5" s="47" t="str">
         <f>Critères!B4</f>
         <v>1.2</v>
@@ -9069,8 +9081,8 @@
       <c r="AMH5" s="14"/>
       <c r="AMI5" s="14"/>
     </row>
-    <row r="6" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
+    <row r="6" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="82"/>
       <c r="B6" s="47" t="str">
         <f>Critères!B5</f>
         <v>1.3</v>
@@ -9145,8 +9157,8 @@
       <c r="BK6" s="2"/>
       <c r="BL6" s="2"/>
     </row>
-    <row r="7" spans="1:1023" ht="60" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
+    <row r="7" spans="1:1023" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="82"/>
       <c r="B7" s="47" t="str">
         <f>Critères!B6</f>
         <v>1.4</v>
@@ -9164,8 +9176,8 @@
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
     </row>
-    <row r="8" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="87"/>
+    <row r="8" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="82"/>
       <c r="B8" s="47" t="str">
         <f>Critères!B7</f>
         <v>1.5</v>
@@ -9183,8 +9195,8 @@
       <c r="F8" s="48"/>
       <c r="G8" s="33"/>
     </row>
-    <row r="9" spans="1:1023" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="87"/>
+    <row r="9" spans="1:1023" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="82"/>
       <c r="B9" s="47" t="str">
         <f>Critères!B8</f>
         <v>1.6</v>
@@ -9202,8 +9214,8 @@
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
     </row>
-    <row r="10" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="87"/>
+    <row r="10" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="82"/>
       <c r="B10" s="47" t="str">
         <f>Critères!B9</f>
         <v>1.7</v>
@@ -9221,7 +9233,7 @@
       <c r="F10" s="33"/>
       <c r="G10" s="33"/>
     </row>
-    <row r="11" spans="1:1023" ht="45.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1023" ht="45.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="61" t="str">
         <f>Critères!$A$10</f>
         <v>CADRES</v>
@@ -9243,8 +9255,8 @@
       <c r="F11" s="49"/>
       <c r="G11" s="33"/>
     </row>
-    <row r="12" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="87" t="str">
+    <row r="12" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="82" t="str">
         <f>Critères!$A$11</f>
         <v>COULEURS</v>
       </c>
@@ -9265,8 +9277,8 @@
       <c r="F12" s="33"/>
       <c r="G12" s="33"/>
     </row>
-    <row r="13" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="87"/>
+    <row r="13" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="82"/>
       <c r="B13" s="47" t="str">
         <f>Critères!B12</f>
         <v>3.2</v>
@@ -9284,8 +9296,8 @@
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
     </row>
-    <row r="14" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="87" t="str">
+    <row r="14" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="82" t="str">
         <f>Critères!$A$13</f>
         <v>MULTIMÉDIA</v>
       </c>
@@ -9306,8 +9318,8 @@
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
     </row>
-    <row r="15" spans="1:1023" ht="60" x14ac:dyDescent="0.2">
-      <c r="A15" s="87"/>
+    <row r="15" spans="1:1023" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="82"/>
       <c r="B15" s="47" t="str">
         <f>Critères!B14</f>
         <v>4.2</v>
@@ -9325,8 +9337,8 @@
       <c r="F15" s="33"/>
       <c r="G15" s="33"/>
     </row>
-    <row r="16" spans="1:1023" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="87"/>
+    <row r="16" spans="1:1023" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="82"/>
       <c r="B16" s="47" t="str">
         <f>Critères!B15</f>
         <v>4.3</v>
@@ -9344,8 +9356,8 @@
       <c r="F16" s="33"/>
       <c r="G16" s="33"/>
     </row>
-    <row r="17" spans="1:64" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="87"/>
+    <row r="17" spans="1:64" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="82"/>
       <c r="B17" s="47" t="str">
         <f>Critères!B16</f>
         <v>4.4</v>
@@ -9363,8 +9375,8 @@
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
     </row>
-    <row r="18" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="87"/>
+    <row r="18" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="82"/>
       <c r="B18" s="47" t="str">
         <f>Critères!B17</f>
         <v>4.8</v>
@@ -9382,8 +9394,8 @@
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
     </row>
-    <row r="19" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="87"/>
+    <row r="19" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="82"/>
       <c r="B19" s="47" t="str">
         <f>Critères!B18</f>
         <v>4.9</v>
@@ -9401,8 +9413,8 @@
       <c r="F19" s="33"/>
       <c r="G19" s="33"/>
     </row>
-    <row r="20" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="87"/>
+    <row r="20" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="82"/>
       <c r="B20" s="47" t="str">
         <f>Critères!B19</f>
         <v>4.10</v>
@@ -9420,8 +9432,8 @@
       <c r="F20" s="33"/>
       <c r="G20" s="33"/>
     </row>
-    <row r="21" spans="1:64" ht="45" x14ac:dyDescent="0.2">
-      <c r="A21" s="87"/>
+    <row r="21" spans="1:64" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="82"/>
       <c r="B21" s="47" t="str">
         <f>Critères!B20</f>
         <v>4.11</v>
@@ -9439,8 +9451,8 @@
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
     </row>
-    <row r="22" spans="1:64" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="87" t="s">
+    <row r="22" spans="1:64" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="82" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="47" t="str">
@@ -9460,8 +9472,8 @@
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
     </row>
-    <row r="23" spans="1:64" ht="45" x14ac:dyDescent="0.2">
-      <c r="A23" s="87"/>
+    <row r="23" spans="1:64" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="82"/>
       <c r="B23" s="47" t="str">
         <f>Critères!B22</f>
         <v>5.7</v>
@@ -9479,8 +9491,8 @@
       <c r="F23" s="33"/>
       <c r="G23" s="33"/>
     </row>
-    <row r="24" spans="1:64" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="87" t="str">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A24" s="82" t="str">
         <f>Critères!$A$23</f>
         <v>LIENS</v>
       </c>
@@ -9501,8 +9513,8 @@
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
     </row>
-    <row r="25" spans="1:64" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="87"/>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A25" s="82"/>
       <c r="B25" s="47" t="str">
         <f>Critères!B24</f>
         <v>6.2</v>
@@ -9520,7 +9532,7 @@
       <c r="F25" s="53"/>
       <c r="G25" s="33"/>
     </row>
-    <row r="26" spans="1:64" ht="42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" ht="41.5" x14ac:dyDescent="0.35">
       <c r="A26" s="61" t="s">
         <v>39</v>
       </c>
@@ -9541,8 +9553,8 @@
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A27" s="88" t="s">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="83" t="s">
         <v>117</v>
       </c>
       <c r="B27" s="47" t="str">
@@ -9559,7 +9571,7 @@
       <c r="E27" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="81"/>
+      <c r="F27" s="77"/>
       <c r="G27" s="33"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -9619,8 +9631,8 @@
       <c r="BK27" s="5"/>
       <c r="BL27" s="5"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="89"/>
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="84"/>
       <c r="B28" s="47" t="str">
         <f>Critères!B27</f>
         <v>8.3</v>
@@ -9635,7 +9647,7 @@
       <c r="E28" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="80"/>
+      <c r="F28" s="76"/>
       <c r="G28" s="33"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -9695,8 +9707,8 @@
       <c r="BK28" s="5"/>
       <c r="BL28" s="5"/>
     </row>
-    <row r="29" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="89"/>
+    <row r="29" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="84"/>
       <c r="B29" s="47" t="str">
         <f>Critères!B28</f>
         <v>8.4</v>
@@ -9714,8 +9726,8 @@
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
     </row>
-    <row r="30" spans="1:64" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="89"/>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A30" s="84"/>
       <c r="B30" s="47" t="str">
         <f>Critères!B29</f>
         <v>8.5</v>
@@ -9733,8 +9745,8 @@
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
     </row>
-    <row r="31" spans="1:64" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="89"/>
+    <row r="31" spans="1:64" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="84"/>
       <c r="B31" s="47" t="str">
         <f>Critères!B30</f>
         <v>8.6</v>
@@ -9752,8 +9764,8 @@
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
     </row>
-    <row r="32" spans="1:64" ht="45" x14ac:dyDescent="0.2">
-      <c r="A32" s="89"/>
+    <row r="32" spans="1:64" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="84"/>
       <c r="B32" s="47" t="str">
         <f>Critères!B31</f>
         <v>8.7</v>
@@ -9771,8 +9783,8 @@
       <c r="F32" s="33"/>
       <c r="G32" s="33"/>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
+    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="85"/>
       <c r="B33" s="47" t="str">
         <f>Critères!B32</f>
         <v>8.8</v>
@@ -9790,8 +9802,8 @@
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="87" t="str">
+    <row r="34" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="82" t="str">
         <f>Critères!$A$33</f>
         <v>STRUCTURATION</v>
       </c>
@@ -9812,8 +9824,8 @@
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
     </row>
-    <row r="35" spans="1:7" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="87"/>
+    <row r="35" spans="1:7" ht="43.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="82"/>
       <c r="B35" s="47" t="str">
         <f>Critères!B34</f>
         <v>9.2</v>
@@ -9831,8 +9843,8 @@
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
     </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A36" s="87" t="s">
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="82" t="s">
         <v>118</v>
       </c>
       <c r="B36" s="47" t="str">
@@ -9852,8 +9864,8 @@
       <c r="F36" s="33"/>
       <c r="G36" s="33"/>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="87"/>
+    <row r="37" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="82"/>
       <c r="B37" s="47" t="str">
         <f>Critères!B36</f>
         <v>10.8</v>
@@ -9871,8 +9883,8 @@
       <c r="F37" s="33"/>
       <c r="G37" s="33"/>
     </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A38" s="87"/>
+    <row r="38" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="82"/>
       <c r="B38" s="47" t="str">
         <f>Critères!B37</f>
         <v>10.9</v>
@@ -9890,8 +9902,8 @@
       <c r="F38" s="33"/>
       <c r="G38" s="33"/>
     </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A39" s="87"/>
+    <row r="39" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="82"/>
       <c r="B39" s="47" t="str">
         <f>Critères!B38</f>
         <v>10.10</v>
@@ -9909,8 +9921,8 @@
       <c r="F39" s="33"/>
       <c r="G39" s="33"/>
     </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.2">
-      <c r="A40" s="87"/>
+    <row r="40" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A40" s="82"/>
       <c r="B40" s="47" t="str">
         <f>Critères!B39</f>
         <v>10.14</v>
@@ -9928,8 +9940,8 @@
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="87" t="str">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="82" t="str">
         <f>Critères!$A$40</f>
         <v>FORMULAIRES</v>
       </c>
@@ -9950,8 +9962,8 @@
       <c r="F41" s="33"/>
       <c r="G41" s="33"/>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="87"/>
+    <row r="42" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="82"/>
       <c r="B42" s="47" t="str">
         <f>Critères!B41</f>
         <v>11.2</v>
@@ -9969,8 +9981,8 @@
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
     </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="87"/>
+    <row r="43" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="82"/>
       <c r="B43" s="47" t="str">
         <f>Critères!B42</f>
         <v>11.5</v>
@@ -9988,8 +10000,8 @@
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="87"/>
+    <row r="44" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="82"/>
       <c r="B44" s="47" t="str">
         <f>Critères!B43</f>
         <v>11.6</v>
@@ -10007,8 +10019,8 @@
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
     </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A45" s="87"/>
+    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="82"/>
       <c r="B45" s="47" t="str">
         <f>Critères!B44</f>
         <v>11.7</v>
@@ -10026,8 +10038,8 @@
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
     </row>
-    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="A46" s="87"/>
+    <row r="46" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="82"/>
       <c r="B46" s="47" t="str">
         <f>Critères!B45</f>
         <v>11.9</v>
@@ -10045,8 +10057,8 @@
       <c r="F46" s="33"/>
       <c r="G46" s="33"/>
     </row>
-    <row r="47" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="87"/>
+    <row r="47" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="82"/>
       <c r="B47" s="47" t="str">
         <f>Critères!B46</f>
         <v>11.10</v>
@@ -10064,8 +10076,8 @@
       <c r="F47" s="33"/>
       <c r="G47" s="33"/>
     </row>
-    <row r="48" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="87" t="s">
+    <row r="48" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="82" t="s">
         <v>64</v>
       </c>
       <c r="B48" s="47" t="str">
@@ -10085,8 +10097,8 @@
       <c r="F48" s="33"/>
       <c r="G48" s="33"/>
     </row>
-    <row r="49" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="87"/>
+    <row r="49" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="82"/>
       <c r="B49" s="47" t="str">
         <f>Critères!B48</f>
         <v>12.7</v>
@@ -10104,8 +10116,8 @@
       <c r="F49" s="33"/>
       <c r="G49" s="33"/>
     </row>
-    <row r="50" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="87"/>
+    <row r="50" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="82"/>
       <c r="B50" s="47" t="str">
         <f>Critères!B49</f>
         <v>12.8</v>
@@ -10123,8 +10135,8 @@
       <c r="F50" s="33"/>
       <c r="G50" s="33"/>
     </row>
-    <row r="51" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="87"/>
+    <row r="51" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="82"/>
       <c r="B51" s="47" t="str">
         <f>Critères!B50</f>
         <v>12.9</v>
@@ -10142,8 +10154,8 @@
       <c r="F51" s="33"/>
       <c r="G51" s="33"/>
     </row>
-    <row r="52" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="87"/>
+    <row r="52" spans="1:7" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="82"/>
       <c r="B52" s="47" t="str">
         <f>Critères!B51</f>
         <v>12.11</v>
@@ -10161,8 +10173,8 @@
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
     </row>
-    <row r="53" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="87" t="str">
+    <row r="53" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="82" t="str">
         <f>Critères!$A$52</f>
         <v>CONSULTATION</v>
       </c>
@@ -10183,8 +10195,8 @@
       <c r="F53" s="33"/>
       <c r="G53" s="33"/>
     </row>
-    <row r="54" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="87"/>
+    <row r="54" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="82"/>
       <c r="B54" s="47" t="str">
         <f>Critères!B53</f>
         <v>13.7</v>
@@ -10202,8 +10214,8 @@
       <c r="F54" s="33"/>
       <c r="G54" s="33"/>
     </row>
-    <row r="55" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="87"/>
+    <row r="55" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="82"/>
       <c r="B55" s="47" t="str">
         <f>Critères!B54</f>
         <v>13.8</v>
@@ -10223,11 +10235,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="A48:A52"/>
-    <mergeCell ref="A53:A55"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="A14:A21"/>
     <mergeCell ref="A22:A23"/>
@@ -10236,6 +10243,11 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A53:A55"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D55">
     <cfRule type="cellIs" dxfId="17" priority="2" operator="equal">
@@ -10260,11 +10272,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D4:D55">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D4:D55" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"C,NC,NA,NT"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4:E55">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4:E55" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"D,N"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -10278,51 +10290,51 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BL55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.21875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="65.44140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="5" customWidth="1"/>
-    <col min="8" max="64" width="9.5546875" style="5"/>
-    <col min="1018" max="1024" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.23046875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="33.07421875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="3.765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3.23046875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="65.4609375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.84375" style="5" customWidth="1"/>
+    <col min="8" max="64" width="9.53515625" style="5"/>
+    <col min="1018" max="1024" width="7.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="str">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A1" s="80" t="str">
         <f>Échantillon!A1</f>
         <v>AUDIT SIMPLIFIÉ – GRILLE D'ÉVALUATION</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="str">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A2" s="89" t="str">
         <f>CONCATENATE(Échantillon!B9," : ",Échantillon!C9)</f>
         <v xml:space="preserve"> : </v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-    </row>
-    <row r="3" spans="1:64" s="51" customFormat="1" ht="61.5" x14ac:dyDescent="0.2">
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+    </row>
+    <row r="3" spans="1:64" s="51" customFormat="1" ht="61.5" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
@@ -10402,8 +10414,8 @@
       <c r="BK3" s="50"/>
       <c r="BL3" s="50"/>
     </row>
-    <row r="4" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="str">
+    <row r="4" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="82" t="str">
         <f>Critères!$A$3</f>
         <v>IMAGES</v>
       </c>
@@ -10479,8 +10491,8 @@
       <c r="BK4" s="50"/>
       <c r="BL4" s="50"/>
     </row>
-    <row r="5" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
+    <row r="5" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="82"/>
       <c r="B5" s="47" t="str">
         <f>Critères!B4</f>
         <v>1.2</v>
@@ -10555,8 +10567,8 @@
       <c r="BK5" s="50"/>
       <c r="BL5" s="50"/>
     </row>
-    <row r="6" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
+    <row r="6" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A6" s="82"/>
       <c r="B6" s="47" t="str">
         <f>Critères!B5</f>
         <v>1.3</v>
@@ -10631,8 +10643,8 @@
       <c r="BK6" s="50"/>
       <c r="BL6" s="50"/>
     </row>
-    <row r="7" spans="1:64" s="51" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
+    <row r="7" spans="1:64" s="51" customFormat="1" ht="72.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="82"/>
       <c r="B7" s="47" t="str">
         <f>Critères!B6</f>
         <v>1.4</v>
@@ -10707,8 +10719,8 @@
       <c r="BK7" s="50"/>
       <c r="BL7" s="50"/>
     </row>
-    <row r="8" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="87"/>
+    <row r="8" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A8" s="82"/>
       <c r="B8" s="47" t="str">
         <f>Critères!B7</f>
         <v>1.5</v>
@@ -10783,8 +10795,8 @@
       <c r="BK8" s="50"/>
       <c r="BL8" s="50"/>
     </row>
-    <row r="9" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="87"/>
+    <row r="9" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A9" s="82"/>
       <c r="B9" s="47" t="str">
         <f>Critères!B8</f>
         <v>1.6</v>
@@ -10859,8 +10871,8 @@
       <c r="BK9" s="50"/>
       <c r="BL9" s="50"/>
     </row>
-    <row r="10" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="87"/>
+    <row r="10" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="82"/>
       <c r="B10" s="47" t="str">
         <f>Critères!B9</f>
         <v>1.7</v>
@@ -10935,8 +10947,8 @@
       <c r="BK10" s="50"/>
       <c r="BL10" s="50"/>
     </row>
-    <row r="11" spans="1:64" s="51" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="79" t="str">
+    <row r="11" spans="1:64" s="51" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="75" t="str">
         <f>Critères!$A$10</f>
         <v>CADRES</v>
       </c>
@@ -11014,8 +11026,8 @@
       <c r="BK11" s="50"/>
       <c r="BL11" s="50"/>
     </row>
-    <row r="12" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="87" t="str">
+    <row r="12" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="82" t="str">
         <f>Critères!$A$11</f>
         <v>COULEURS</v>
       </c>
@@ -11093,8 +11105,8 @@
       <c r="BK12" s="50"/>
       <c r="BL12" s="50"/>
     </row>
-    <row r="13" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A13" s="87"/>
+    <row r="13" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A13" s="82"/>
       <c r="B13" s="47" t="str">
         <f>Critères!B12</f>
         <v>3.2</v>
@@ -11169,8 +11181,8 @@
       <c r="BK13" s="50"/>
       <c r="BL13" s="50"/>
     </row>
-    <row r="14" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87" t="str">
+    <row r="14" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="82" t="str">
         <f>Critères!$A$13</f>
         <v>MULTIMÉDIA</v>
       </c>
@@ -11248,8 +11260,8 @@
       <c r="BK14" s="50"/>
       <c r="BL14" s="50"/>
     </row>
-    <row r="15" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A15" s="87"/>
+    <row r="15" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A15" s="82"/>
       <c r="B15" s="47" t="str">
         <f>Critères!B14</f>
         <v>4.2</v>
@@ -11324,8 +11336,8 @@
       <c r="BK15" s="50"/>
       <c r="BL15" s="50"/>
     </row>
-    <row r="16" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="87"/>
+    <row r="16" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="82"/>
       <c r="B16" s="47" t="str">
         <f>Critères!B15</f>
         <v>4.3</v>
@@ -11400,8 +11412,8 @@
       <c r="BK16" s="50"/>
       <c r="BL16" s="50"/>
     </row>
-    <row r="17" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="87"/>
+    <row r="17" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A17" s="82"/>
       <c r="B17" s="47" t="str">
         <f>Critères!B16</f>
         <v>4.4</v>
@@ -11476,8 +11488,8 @@
       <c r="BK17" s="50"/>
       <c r="BL17" s="50"/>
     </row>
-    <row r="18" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A18" s="87"/>
+    <row r="18" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="82"/>
       <c r="B18" s="47" t="str">
         <f>Critères!B17</f>
         <v>4.8</v>
@@ -11552,8 +11564,8 @@
       <c r="BK18" s="50"/>
       <c r="BL18" s="50"/>
     </row>
-    <row r="19" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="87"/>
+    <row r="19" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="82"/>
       <c r="B19" s="47" t="str">
         <f>Critères!B18</f>
         <v>4.9</v>
@@ -11628,8 +11640,8 @@
       <c r="BK19" s="50"/>
       <c r="BL19" s="50"/>
     </row>
-    <row r="20" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="87"/>
+    <row r="20" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A20" s="82"/>
       <c r="B20" s="47" t="str">
         <f>Critères!B19</f>
         <v>4.10</v>
@@ -11704,8 +11716,8 @@
       <c r="BK20" s="50"/>
       <c r="BL20" s="50"/>
     </row>
-    <row r="21" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A21" s="87"/>
+    <row r="21" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="82"/>
       <c r="B21" s="47" t="str">
         <f>Critères!B20</f>
         <v>4.11</v>
@@ -11780,8 +11792,8 @@
       <c r="BK21" s="50"/>
       <c r="BL21" s="50"/>
     </row>
-    <row r="22" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="87" t="s">
+    <row r="22" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="82" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="47" t="str">
@@ -11858,8 +11870,8 @@
       <c r="BK22" s="50"/>
       <c r="BL22" s="50"/>
     </row>
-    <row r="23" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A23" s="87"/>
+    <row r="23" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A23" s="82"/>
       <c r="B23" s="47" t="str">
         <f>Critères!B22</f>
         <v>5.7</v>
@@ -11934,8 +11946,8 @@
       <c r="BK23" s="50"/>
       <c r="BL23" s="50"/>
     </row>
-    <row r="24" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="87" t="str">
+    <row r="24" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="82" t="str">
         <f>Critères!$A$23</f>
         <v>LIENS</v>
       </c>
@@ -12013,8 +12025,8 @@
       <c r="BK24" s="50"/>
       <c r="BL24" s="50"/>
     </row>
-    <row r="25" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="87"/>
+    <row r="25" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A25" s="82"/>
       <c r="B25" s="47" t="str">
         <f>Critères!B24</f>
         <v>6.2</v>
@@ -12089,8 +12101,8 @@
       <c r="BK25" s="50"/>
       <c r="BL25" s="50"/>
     </row>
-    <row r="26" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A26" s="79" t="s">
+    <row r="26" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="75" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="47" t="str">
@@ -12167,8 +12179,8 @@
       <c r="BK26" s="50"/>
       <c r="BL26" s="50"/>
     </row>
-    <row r="27" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A27" s="88" t="s">
+    <row r="27" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="83" t="s">
         <v>117</v>
       </c>
       <c r="B27" s="47" t="str">
@@ -12245,8 +12257,8 @@
       <c r="BK27" s="50"/>
       <c r="BL27" s="50"/>
     </row>
-    <row r="28" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="89"/>
+    <row r="28" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A28" s="84"/>
       <c r="B28" s="47" t="str">
         <f>Critères!B27</f>
         <v>8.3</v>
@@ -12321,8 +12333,8 @@
       <c r="BK28" s="50"/>
       <c r="BL28" s="50"/>
     </row>
-    <row r="29" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="89"/>
+    <row r="29" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A29" s="84"/>
       <c r="B29" s="47" t="str">
         <f>Critères!B28</f>
         <v>8.4</v>
@@ -12397,8 +12409,8 @@
       <c r="BK29" s="50"/>
       <c r="BL29" s="50"/>
     </row>
-    <row r="30" spans="1:64" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="89"/>
+    <row r="30" spans="1:64" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="84"/>
       <c r="B30" s="47" t="str">
         <f>Critères!B29</f>
         <v>8.5</v>
@@ -12473,8 +12485,8 @@
       <c r="BK30" s="50"/>
       <c r="BL30" s="50"/>
     </row>
-    <row r="31" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="89"/>
+    <row r="31" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A31" s="84"/>
       <c r="B31" s="47" t="str">
         <f>Critères!B30</f>
         <v>8.6</v>
@@ -12549,8 +12561,8 @@
       <c r="BK31" s="50"/>
       <c r="BL31" s="50"/>
     </row>
-    <row r="32" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A32" s="89"/>
+    <row r="32" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="84"/>
       <c r="B32" s="47" t="str">
         <f>Critères!B31</f>
         <v>8.7</v>
@@ -12625,8 +12637,8 @@
       <c r="BK32" s="50"/>
       <c r="BL32" s="50"/>
     </row>
-    <row r="33" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
+    <row r="33" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="85"/>
       <c r="B33" s="47" t="str">
         <f>Critères!B32</f>
         <v>8.8</v>
@@ -12701,8 +12713,8 @@
       <c r="BK33" s="50"/>
       <c r="BL33" s="50"/>
     </row>
-    <row r="34" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="87" t="str">
+    <row r="34" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="82" t="str">
         <f>Critères!$A$33</f>
         <v>STRUCTURATION</v>
       </c>
@@ -12780,8 +12792,8 @@
       <c r="BK34" s="50"/>
       <c r="BL34" s="50"/>
     </row>
-    <row r="35" spans="1:64" s="51" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="87"/>
+    <row r="35" spans="1:64" s="51" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="82"/>
       <c r="B35" s="47" t="str">
         <f>Critères!B34</f>
         <v>9.2</v>
@@ -12856,8 +12868,8 @@
       <c r="BK35" s="50"/>
       <c r="BL35" s="50"/>
     </row>
-    <row r="36" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="87" t="s">
+    <row r="36" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="82" t="s">
         <v>118</v>
       </c>
       <c r="B36" s="47" t="str">
@@ -12934,8 +12946,8 @@
       <c r="BK36" s="50"/>
       <c r="BL36" s="50"/>
     </row>
-    <row r="37" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="87"/>
+    <row r="37" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="82"/>
       <c r="B37" s="47" t="str">
         <f>Critères!B36</f>
         <v>10.8</v>
@@ -13010,8 +13022,8 @@
       <c r="BK37" s="50"/>
       <c r="BL37" s="50"/>
     </row>
-    <row r="38" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A38" s="87"/>
+    <row r="38" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A38" s="82"/>
       <c r="B38" s="47" t="str">
         <f>Critères!B37</f>
         <v>10.9</v>
@@ -13086,8 +13098,8 @@
       <c r="BK38" s="50"/>
       <c r="BL38" s="50"/>
     </row>
-    <row r="39" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A39" s="87"/>
+    <row r="39" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A39" s="82"/>
       <c r="B39" s="47" t="str">
         <f>Critères!B38</f>
         <v>10.10</v>
@@ -13162,8 +13174,8 @@
       <c r="BK39" s="50"/>
       <c r="BL39" s="50"/>
     </row>
-    <row r="40" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A40" s="87"/>
+    <row r="40" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A40" s="82"/>
       <c r="B40" s="47" t="str">
         <f>Critères!B39</f>
         <v>10.14</v>
@@ -13238,8 +13250,8 @@
       <c r="BK40" s="50"/>
       <c r="BL40" s="50"/>
     </row>
-    <row r="41" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="87" t="str">
+    <row r="41" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="82" t="str">
         <f>Critères!$A$40</f>
         <v>FORMULAIRES</v>
       </c>
@@ -13317,8 +13329,8 @@
       <c r="BK41" s="50"/>
       <c r="BL41" s="50"/>
     </row>
-    <row r="42" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A42" s="87"/>
+    <row r="42" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="82"/>
       <c r="B42" s="47" t="str">
         <f>Critères!B41</f>
         <v>11.2</v>
@@ -13393,8 +13405,8 @@
       <c r="BK42" s="50"/>
       <c r="BL42" s="50"/>
     </row>
-    <row r="43" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="87"/>
+    <row r="43" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="82"/>
       <c r="B43" s="47" t="str">
         <f>Critères!B42</f>
         <v>11.5</v>
@@ -13469,8 +13481,8 @@
       <c r="BK43" s="50"/>
       <c r="BL43" s="50"/>
     </row>
-    <row r="44" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A44" s="87"/>
+    <row r="44" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="82"/>
       <c r="B44" s="47" t="str">
         <f>Critères!B43</f>
         <v>11.6</v>
@@ -13545,8 +13557,8 @@
       <c r="BK44" s="50"/>
       <c r="BL44" s="50"/>
     </row>
-    <row r="45" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A45" s="87"/>
+    <row r="45" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="82"/>
       <c r="B45" s="47" t="str">
         <f>Critères!B44</f>
         <v>11.7</v>
@@ -13621,8 +13633,8 @@
       <c r="BK45" s="50"/>
       <c r="BL45" s="50"/>
     </row>
-    <row r="46" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A46" s="87"/>
+    <row r="46" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="82"/>
       <c r="B46" s="47" t="str">
         <f>Critères!B45</f>
         <v>11.9</v>
@@ -13697,8 +13709,8 @@
       <c r="BK46" s="50"/>
       <c r="BL46" s="50"/>
     </row>
-    <row r="47" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A47" s="87"/>
+    <row r="47" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="82"/>
       <c r="B47" s="47" t="str">
         <f>Critères!B46</f>
         <v>11.10</v>
@@ -13773,8 +13785,8 @@
       <c r="BK47" s="50"/>
       <c r="BL47" s="50"/>
     </row>
-    <row r="48" spans="1:64" s="51" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A48" s="87" t="s">
+    <row r="48" spans="1:64" s="51" customFormat="1" ht="87" x14ac:dyDescent="0.3">
+      <c r="A48" s="82" t="s">
         <v>64</v>
       </c>
       <c r="B48" s="47" t="str">
@@ -13851,8 +13863,8 @@
       <c r="BK48" s="50"/>
       <c r="BL48" s="50"/>
     </row>
-    <row r="49" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A49" s="87"/>
+    <row r="49" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A49" s="82"/>
       <c r="B49" s="47" t="str">
         <f>Critères!B48</f>
         <v>12.7</v>
@@ -13927,8 +13939,8 @@
       <c r="BK49" s="50"/>
       <c r="BL49" s="50"/>
     </row>
-    <row r="50" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="87"/>
+    <row r="50" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A50" s="82"/>
       <c r="B50" s="47" t="str">
         <f>Critères!B49</f>
         <v>12.8</v>
@@ -14003,8 +14015,8 @@
       <c r="BK50" s="50"/>
       <c r="BL50" s="50"/>
     </row>
-    <row r="51" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="87"/>
+    <row r="51" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="82"/>
       <c r="B51" s="47" t="str">
         <f>Critères!B50</f>
         <v>12.9</v>
@@ -14079,8 +14091,8 @@
       <c r="BK51" s="50"/>
       <c r="BL51" s="50"/>
     </row>
-    <row r="52" spans="1:64" s="51" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A52" s="87"/>
+    <row r="52" spans="1:64" s="51" customFormat="1" ht="72.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="82"/>
       <c r="B52" s="47" t="str">
         <f>Critères!B51</f>
         <v>12.11</v>
@@ -14155,8 +14167,8 @@
       <c r="BK52" s="50"/>
       <c r="BL52" s="50"/>
     </row>
-    <row r="53" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="87" t="str">
+    <row r="53" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="82" t="str">
         <f>Critères!$A$52</f>
         <v>CONSULTATION</v>
       </c>
@@ -14234,8 +14246,8 @@
       <c r="BK53" s="50"/>
       <c r="BL53" s="50"/>
     </row>
-    <row r="54" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A54" s="87"/>
+    <row r="54" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A54" s="82"/>
       <c r="B54" s="47" t="str">
         <f>Critères!B53</f>
         <v>13.7</v>
@@ -14310,8 +14322,8 @@
       <c r="BK54" s="50"/>
       <c r="BL54" s="50"/>
     </row>
-    <row r="55" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A55" s="87"/>
+    <row r="55" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="82"/>
       <c r="B55" s="47" t="str">
         <f>Critères!B54</f>
         <v>13.8</v>
@@ -14388,12 +14400,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="A48:A52"/>
     <mergeCell ref="A14:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
@@ -14401,6 +14407,12 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A48:A52"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D55">
     <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
@@ -14425,11 +14437,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D4:D55">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D4:D55" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"C,NC,NA,NT"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4:E55">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4:E55" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"D,N"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -14443,51 +14455,51 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:BL55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.21875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="3.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="62.21875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" style="5" customWidth="1"/>
-    <col min="8" max="64" width="9.5546875" style="5"/>
-    <col min="1018" max="1024" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.23046875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="33.07421875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="3.765625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3.23046875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="62.23046875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.84375" style="5" customWidth="1"/>
+    <col min="8" max="64" width="9.53515625" style="5"/>
+    <col min="1018" max="1024" width="7.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="84" t="str">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A1" s="80" t="str">
         <f>Échantillon!A1</f>
         <v>AUDIT SIMPLIFIÉ – GRILLE D'ÉVALUATION</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="str">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
+      <c r="A2" s="89" t="str">
         <f>CONCATENATE(Échantillon!B10," : ",Échantillon!C10)</f>
         <v xml:space="preserve"> : </v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-    </row>
-    <row r="3" spans="1:64" s="51" customFormat="1" ht="61.5" x14ac:dyDescent="0.2">
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+    </row>
+    <row r="3" spans="1:64" s="51" customFormat="1" ht="61.5" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>8</v>
       </c>
@@ -14567,8 +14579,8 @@
       <c r="BK3" s="50"/>
       <c r="BL3" s="50"/>
     </row>
-    <row r="4" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="str">
+    <row r="4" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="82" t="str">
         <f>Critères!$A$3</f>
         <v>IMAGES</v>
       </c>
@@ -14645,8 +14657,8 @@
       <c r="BK4" s="50"/>
       <c r="BL4" s="50"/>
     </row>
-    <row r="5" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
+    <row r="5" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="82"/>
       <c r="B5" s="47" t="str">
         <f>Critères!B4</f>
         <v>1.2</v>
@@ -14721,8 +14733,8 @@
       <c r="BK5" s="50"/>
       <c r="BL5" s="50"/>
     </row>
-    <row r="6" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
+    <row r="6" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A6" s="82"/>
       <c r="B6" s="47" t="str">
         <f>Critères!B5</f>
         <v>1.3</v>
@@ -14797,8 +14809,8 @@
       <c r="BK6" s="50"/>
       <c r="BL6" s="50"/>
     </row>
-    <row r="7" spans="1:64" s="51" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A7" s="87"/>
+    <row r="7" spans="1:64" s="51" customFormat="1" ht="72.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="82"/>
       <c r="B7" s="47" t="str">
         <f>Critères!B6</f>
         <v>1.4</v>
@@ -14873,8 +14885,8 @@
       <c r="BK7" s="50"/>
       <c r="BL7" s="50"/>
     </row>
-    <row r="8" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A8" s="87"/>
+    <row r="8" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A8" s="82"/>
       <c r="B8" s="47" t="str">
         <f>Critères!B7</f>
         <v>1.5</v>
@@ -14949,8 +14961,8 @@
       <c r="BK8" s="50"/>
       <c r="BL8" s="50"/>
     </row>
-    <row r="9" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="87"/>
+    <row r="9" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A9" s="82"/>
       <c r="B9" s="47" t="str">
         <f>Critères!B8</f>
         <v>1.6</v>
@@ -15025,8 +15037,8 @@
       <c r="BK9" s="50"/>
       <c r="BL9" s="50"/>
     </row>
-    <row r="10" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="87"/>
+    <row r="10" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="82"/>
       <c r="B10" s="47" t="str">
         <f>Critères!B9</f>
         <v>1.7</v>
@@ -15101,8 +15113,8 @@
       <c r="BK10" s="50"/>
       <c r="BL10" s="50"/>
     </row>
-    <row r="11" spans="1:64" s="51" customFormat="1" ht="41.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="79" t="str">
+    <row r="11" spans="1:64" s="51" customFormat="1" ht="41" x14ac:dyDescent="0.3">
+      <c r="A11" s="75" t="str">
         <f>Critères!$A$10</f>
         <v>CADRES</v>
       </c>
@@ -15180,8 +15192,8 @@
       <c r="BK11" s="50"/>
       <c r="BL11" s="50"/>
     </row>
-    <row r="12" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="87" t="str">
+    <row r="12" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="82" t="str">
         <f>Critères!$A$11</f>
         <v>COULEURS</v>
       </c>
@@ -15259,8 +15271,8 @@
       <c r="BK12" s="50"/>
       <c r="BL12" s="50"/>
     </row>
-    <row r="13" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A13" s="87"/>
+    <row r="13" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A13" s="82"/>
       <c r="B13" s="47" t="str">
         <f>Critères!B12</f>
         <v>3.2</v>
@@ -15335,8 +15347,8 @@
       <c r="BK13" s="50"/>
       <c r="BL13" s="50"/>
     </row>
-    <row r="14" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="87" t="str">
+    <row r="14" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="82" t="str">
         <f>Critères!$A$13</f>
         <v>MULTIMÉDIA</v>
       </c>
@@ -15414,8 +15426,8 @@
       <c r="BK14" s="50"/>
       <c r="BL14" s="50"/>
     </row>
-    <row r="15" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A15" s="87"/>
+    <row r="15" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A15" s="82"/>
       <c r="B15" s="47" t="str">
         <f>Critères!B14</f>
         <v>4.2</v>
@@ -15490,8 +15502,8 @@
       <c r="BK15" s="50"/>
       <c r="BL15" s="50"/>
     </row>
-    <row r="16" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="87"/>
+    <row r="16" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="82"/>
       <c r="B16" s="47" t="str">
         <f>Critères!B15</f>
         <v>4.3</v>
@@ -15566,8 +15578,8 @@
       <c r="BK16" s="50"/>
       <c r="BL16" s="50"/>
     </row>
-    <row r="17" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="87"/>
+    <row r="17" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A17" s="82"/>
       <c r="B17" s="47" t="str">
         <f>Critères!B16</f>
         <v>4.4</v>
@@ -15642,8 +15654,8 @@
       <c r="BK17" s="50"/>
       <c r="BL17" s="50"/>
     </row>
-    <row r="18" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A18" s="87"/>
+    <row r="18" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="82"/>
       <c r="B18" s="47" t="str">
         <f>Critères!B17</f>
         <v>4.8</v>
@@ -15718,8 +15730,8 @@
       <c r="BK18" s="50"/>
       <c r="BL18" s="50"/>
     </row>
-    <row r="19" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="87"/>
+    <row r="19" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="82"/>
       <c r="B19" s="47" t="str">
         <f>Critères!B18</f>
         <v>4.9</v>
@@ -15794,8 +15806,8 @@
       <c r="BK19" s="50"/>
       <c r="BL19" s="50"/>
     </row>
-    <row r="20" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="87"/>
+    <row r="20" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A20" s="82"/>
       <c r="B20" s="47" t="str">
         <f>Critères!B19</f>
         <v>4.10</v>
@@ -15870,8 +15882,8 @@
       <c r="BK20" s="50"/>
       <c r="BL20" s="50"/>
     </row>
-    <row r="21" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A21" s="87"/>
+    <row r="21" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="82"/>
       <c r="B21" s="47" t="str">
         <f>Critères!B20</f>
         <v>4.11</v>
@@ -15946,8 +15958,8 @@
       <c r="BK21" s="50"/>
       <c r="BL21" s="50"/>
     </row>
-    <row r="22" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="87" t="s">
+    <row r="22" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="82" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="47" t="str">
@@ -16024,8 +16036,8 @@
       <c r="BK22" s="50"/>
       <c r="BL22" s="50"/>
     </row>
-    <row r="23" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A23" s="87"/>
+    <row r="23" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A23" s="82"/>
       <c r="B23" s="47" t="str">
         <f>Critères!B22</f>
         <v>5.7</v>
@@ -16100,8 +16112,8 @@
       <c r="BK23" s="50"/>
       <c r="BL23" s="50"/>
     </row>
-    <row r="24" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="87" t="str">
+    <row r="24" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="82" t="str">
         <f>Critères!$A$23</f>
         <v>LIENS</v>
       </c>
@@ -16179,8 +16191,8 @@
       <c r="BK24" s="50"/>
       <c r="BL24" s="50"/>
     </row>
-    <row r="25" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="87"/>
+    <row r="25" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A25" s="82"/>
       <c r="B25" s="47" t="str">
         <f>Critères!B24</f>
         <v>6.2</v>
@@ -16255,8 +16267,8 @@
       <c r="BK25" s="50"/>
       <c r="BL25" s="50"/>
     </row>
-    <row r="26" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A26" s="79" t="s">
+    <row r="26" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="75" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="47" t="str">
@@ -16333,8 +16345,8 @@
       <c r="BK26" s="50"/>
       <c r="BL26" s="50"/>
     </row>
-    <row r="27" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A27" s="88" t="s">
+    <row r="27" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="83" t="s">
         <v>117</v>
       </c>
       <c r="B27" s="47" t="str">
@@ -16351,7 +16363,7 @@
       <c r="E27" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="81"/>
+      <c r="F27" s="77"/>
       <c r="G27" s="33"/>
       <c r="H27" s="50"/>
       <c r="I27" s="50"/>
@@ -16411,8 +16423,8 @@
       <c r="BK27" s="50"/>
       <c r="BL27" s="50"/>
     </row>
-    <row r="28" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="89"/>
+    <row r="28" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A28" s="84"/>
       <c r="B28" s="47" t="str">
         <f>Critères!B27</f>
         <v>8.3</v>
@@ -16487,8 +16499,8 @@
       <c r="BK28" s="50"/>
       <c r="BL28" s="50"/>
     </row>
-    <row r="29" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="89"/>
+    <row r="29" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A29" s="84"/>
       <c r="B29" s="47" t="str">
         <f>Critères!B28</f>
         <v>8.4</v>
@@ -16563,8 +16575,8 @@
       <c r="BK29" s="50"/>
       <c r="BL29" s="50"/>
     </row>
-    <row r="30" spans="1:64" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="89"/>
+    <row r="30" spans="1:64" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="84"/>
       <c r="B30" s="47" t="str">
         <f>Critères!B29</f>
         <v>8.5</v>
@@ -16639,8 +16651,8 @@
       <c r="BK30" s="50"/>
       <c r="BL30" s="50"/>
     </row>
-    <row r="31" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="89"/>
+    <row r="31" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A31" s="84"/>
       <c r="B31" s="47" t="str">
         <f>Critères!B30</f>
         <v>8.6</v>
@@ -16715,8 +16727,8 @@
       <c r="BK31" s="50"/>
       <c r="BL31" s="50"/>
     </row>
-    <row r="32" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A32" s="89"/>
+    <row r="32" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="84"/>
       <c r="B32" s="47" t="str">
         <f>Critères!B31</f>
         <v>8.7</v>
@@ -16791,8 +16803,8 @@
       <c r="BK32" s="50"/>
       <c r="BL32" s="50"/>
     </row>
-    <row r="33" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
+    <row r="33" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="85"/>
       <c r="B33" s="47" t="str">
         <f>Critères!B32</f>
         <v>8.8</v>
@@ -16867,8 +16879,8 @@
       <c r="BK33" s="50"/>
       <c r="BL33" s="50"/>
     </row>
-    <row r="34" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="87" t="str">
+    <row r="34" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="82" t="str">
         <f>Critères!$A$33</f>
         <v>STRUCTURATION</v>
       </c>
@@ -16946,8 +16958,8 @@
       <c r="BK34" s="50"/>
       <c r="BL34" s="50"/>
     </row>
-    <row r="35" spans="1:64" s="51" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="87"/>
+    <row r="35" spans="1:64" s="51" customFormat="1" ht="54.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="82"/>
       <c r="B35" s="47" t="str">
         <f>Critères!B34</f>
         <v>9.2</v>
@@ -17022,8 +17034,8 @@
       <c r="BK35" s="50"/>
       <c r="BL35" s="50"/>
     </row>
-    <row r="36" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="87" t="s">
+    <row r="36" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A36" s="82" t="s">
         <v>118</v>
       </c>
       <c r="B36" s="47" t="str">
@@ -17100,8 +17112,8 @@
       <c r="BK36" s="50"/>
       <c r="BL36" s="50"/>
     </row>
-    <row r="37" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="87"/>
+    <row r="37" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A37" s="82"/>
       <c r="B37" s="47" t="str">
         <f>Critères!B36</f>
         <v>10.8</v>
@@ -17176,8 +17188,8 @@
       <c r="BK37" s="50"/>
       <c r="BL37" s="50"/>
     </row>
-    <row r="38" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A38" s="87"/>
+    <row r="38" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A38" s="82"/>
       <c r="B38" s="47" t="str">
         <f>Critères!B37</f>
         <v>10.9</v>
@@ -17252,8 +17264,8 @@
       <c r="BK38" s="50"/>
       <c r="BL38" s="50"/>
     </row>
-    <row r="39" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A39" s="87"/>
+    <row r="39" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A39" s="82"/>
       <c r="B39" s="47" t="str">
         <f>Critères!B38</f>
         <v>10.10</v>
@@ -17328,8 +17340,8 @@
       <c r="BK39" s="50"/>
       <c r="BL39" s="50"/>
     </row>
-    <row r="40" spans="1:64" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A40" s="87"/>
+    <row r="40" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A40" s="82"/>
       <c r="B40" s="47" t="str">
         <f>Critères!B39</f>
         <v>10.14</v>
@@ -17404,8 +17416,8 @@
       <c r="BK40" s="50"/>
       <c r="BL40" s="50"/>
     </row>
-    <row r="41" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="87" t="str">
+    <row r="41" spans="1:64" s="51" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="82" t="str">
         <f>Critères!$A$40</f>
         <v>FORMULAIRES</v>
       </c>
@@ -17483,8 +17495,8 @@
       <c r="BK41" s="50"/>
       <c r="BL41" s="50"/>
     </row>
-    <row r="42" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A42" s="87"/>
+    <row r="42" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="82"/>
       <c r="B42" s="47" t="str">
         <f>Critères!B41</f>
         <v>11.2</v>
@@ -17559,8 +17571,8 @@
       <c r="BK42" s="50"/>
       <c r="BL42" s="50"/>
     </row>
-    <row r="43" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A43" s="87"/>
+    <row r="43" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A43" s="82"/>
       <c r="B43" s="47" t="str">
         <f>Critères!B42</f>
         <v>11.5</v>
@@ -17635,8 +17647,8 @@
       <c r="BK43" s="50"/>
       <c r="BL43" s="50"/>
     </row>
-    <row r="44" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A44" s="87"/>
+    <row r="44" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="82"/>
       <c r="B44" s="47" t="str">
         <f>Critères!B43</f>
         <v>11.6</v>
@@ -17711,8 +17723,8 @@
       <c r="BK44" s="50"/>
       <c r="BL44" s="50"/>
     </row>
-    <row r="45" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A45" s="87"/>
+    <row r="45" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="82"/>
       <c r="B45" s="47" t="str">
         <f>Critères!B44</f>
         <v>11.7</v>
@@ -17787,8 +17799,8 @@
       <c r="BK45" s="50"/>
       <c r="BL45" s="50"/>
     </row>
-    <row r="46" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A46" s="87"/>
+    <row r="46" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A46" s="82"/>
       <c r="B46" s="47" t="str">
         <f>Critères!B45</f>
         <v>11.9</v>
@@ -17863,8 +17875,8 @@
       <c r="BK46" s="50"/>
       <c r="BL46" s="50"/>
     </row>
-    <row r="47" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A47" s="87"/>
+    <row r="47" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A47" s="82"/>
       <c r="B47" s="47" t="str">
         <f>Critères!B46</f>
         <v>11.10</v>
@@ -17939,8 +17951,8 @@
       <c r="BK47" s="50"/>
       <c r="BL47" s="50"/>
     </row>
-    <row r="48" spans="1:64" s="51" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A48" s="87" t="s">
+    <row r="48" spans="1:64" s="51" customFormat="1" ht="87" x14ac:dyDescent="0.3">
+      <c r="A48" s="82" t="s">
         <v>64</v>
       </c>
       <c r="B48" s="47" t="str">
@@ -18017,8 +18029,8 @@
       <c r="BK48" s="50"/>
       <c r="BL48" s="50"/>
     </row>
-    <row r="49" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A49" s="87"/>
+    <row r="49" spans="1:64" s="51" customFormat="1" ht="58" x14ac:dyDescent="0.3">
+      <c r="A49" s="82"/>
       <c r="B49" s="47" t="str">
         <f>Critères!B48</f>
         <v>12.7</v>
@@ -18093,8 +18105,8 @@
       <c r="BK49" s="50"/>
       <c r="BL49" s="50"/>
     </row>
-    <row r="50" spans="1:64" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="87"/>
+    <row r="50" spans="1:64" s="51" customFormat="1" ht="29" x14ac:dyDescent="0.3">
+      <c r="A50" s="82"/>
       <c r="B50" s="47" t="str">
         <f>Critères!B49</f>
         <v>12.8</v>
@@ -18169,8 +18181,8 @@
       <c r="BK50" s="50"/>
       <c r="BL50" s="50"/>
     </row>
-    <row r="51" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="87"/>
+    <row r="51" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A51" s="82"/>
       <c r="B51" s="47" t="str">
         <f>Critères!B50</f>
         <v>12.9</v>
@@ -18245,8 +18257,8 @@
       <c r="BK51" s="50"/>
       <c r="BL51" s="50"/>
     </row>
-    <row r="52" spans="1:64" s="51" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A52" s="87"/>
+    <row r="52" spans="1:64" s="51" customFormat="1" ht="72.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="82"/>
       <c r="B52" s="47" t="str">
         <f>Critères!B51</f>
         <v>12.11</v>
@@ -18321,8 +18333,8 @@
       <c r="BK52" s="50"/>
       <c r="BL52" s="50"/>
     </row>
-    <row r="53" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="87" t="str">
+    <row r="53" spans="1:64" s="51" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="82" t="str">
         <f>Critères!$A$52</f>
         <v>CONSULTATION</v>
       </c>
@@ -18400,8 +18412,8 @@
       <c r="BK53" s="50"/>
       <c r="BL53" s="50"/>
     </row>
-    <row r="54" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A54" s="87"/>
+    <row r="54" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A54" s="82"/>
       <c r="B54" s="47" t="str">
         <f>Critères!B53</f>
         <v>13.7</v>
@@ -18476,8 +18488,8 @@
       <c r="BK54" s="50"/>
       <c r="BL54" s="50"/>
     </row>
-    <row r="55" spans="1:64" s="51" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A55" s="87"/>
+    <row r="55" spans="1:64" s="51" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+      <c r="A55" s="82"/>
       <c r="B55" s="47" t="str">
         <f>Critères!B54</f>
         <v>13.8</v>
@@ -18554,12 +18566,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="A48:A52"/>
     <mergeCell ref="A14:A21"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A24:A25"/>
@@ -18567,6 +18573,12 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A48:A52"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D55">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
@@ -18591,11 +18603,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D4:D55">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D4:D55" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"C,NC,NA,NT"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4:E55">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="E4:E55" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"D,N"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>